<commit_message>
- Some restructuring - Finished user evaluation section
</commit_message>
<xml_diff>
--- a/Figures/User Evaluation Results.xlsx
+++ b/Figures/User Evaluation Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCB\Desktop\Bachelor Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repos\Vitrivr VR Thesis\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7390F34C-3C03-46B9-8696-84744BFC3E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D6CF37-5AF0-49E2-BE27-FBE5663FED5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{6BF3DCD3-A42B-4BDB-84D3-BFEA7022B683}"/>
   </bookViews>
@@ -811,7 +811,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="25"/>
         <c:overlap val="100"/>
         <c:axId val="694170696"/>
         <c:axId val="694172008"/>
@@ -1729,7 +1729,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="25"/>
         <c:overlap val="100"/>
         <c:axId val="697222088"/>
         <c:axId val="697221760"/>
@@ -2978,15 +2978,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>627529</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>113179</xdr:rowOff>
+      <xdr:colOff>157062</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113176</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>728382</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>189379</xdr:rowOff>
+      <xdr:colOff>257915</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179613</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3013,16 +3013,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>621924</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>146797</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>75256</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>160744</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>235743</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>2742</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3349,8 +3349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42140BE7-5336-4D7F-9905-53D88C40A621}">
   <dimension ref="C5:AG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AF50" sqref="AF50"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,6 +3460,10 @@
       <c r="Q6">
         <v>3</v>
       </c>
+      <c r="R6">
+        <f>ROUND(AVERAGE(D6:Q6),2)</f>
+        <v>2.86</v>
+      </c>
       <c r="T6" t="s">
         <v>0</v>
       </c>
@@ -3530,6 +3534,10 @@
       <c r="Q7">
         <v>4</v>
       </c>
+      <c r="R7">
+        <f>ROUND(AVERAGE(D7:Q7),2)</f>
+        <v>1.79</v>
+      </c>
       <c r="T7" t="s">
         <v>1</v>
       </c>
@@ -3614,6 +3622,10 @@
       </c>
       <c r="Q8">
         <v>1</v>
+      </c>
+      <c r="R8">
+        <f>ROUND(AVERAGE(D8:Q8),2)</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="AB8" t="s">
         <v>2</v>
@@ -3685,6 +3697,10 @@
       <c r="Q9">
         <v>2</v>
       </c>
+      <c r="R9">
+        <f>ROUND(AVERAGE(D9:Q9),2)</f>
+        <v>1.36</v>
+      </c>
       <c r="AB9" t="s">
         <v>3</v>
       </c>
@@ -3755,6 +3771,10 @@
       <c r="Q10">
         <v>2</v>
       </c>
+      <c r="R10">
+        <f>ROUND(AVERAGE(D10:Q10),2)</f>
+        <v>1.5</v>
+      </c>
       <c r="AB10" t="s">
         <v>4</v>
       </c>
@@ -3825,6 +3845,10 @@
       <c r="Q11">
         <v>1</v>
       </c>
+      <c r="R11">
+        <f>ROUND(AVERAGE(D11:Q11),2)</f>
+        <v>1.36</v>
+      </c>
       <c r="AB11" t="s">
         <v>5</v>
       </c>
@@ -3895,6 +3919,10 @@
       <c r="Q12">
         <v>4</v>
       </c>
+      <c r="R12">
+        <f>ROUND(AVERAGE(D12:Q12),2)</f>
+        <v>2</v>
+      </c>
       <c r="AB12" t="s">
         <v>6</v>
       </c>
@@ -3965,6 +3993,10 @@
       <c r="Q13">
         <v>3</v>
       </c>
+      <c r="R13">
+        <f>ROUND(AVERAGE(D13:Q13),2)</f>
+        <v>2.4300000000000002</v>
+      </c>
       <c r="AB13" t="s">
         <v>7</v>
       </c>
@@ -4035,6 +4067,10 @@
       <c r="Q14">
         <v>1</v>
       </c>
+      <c r="R14">
+        <f>ROUND(AVERAGE(D14:Q14),2)</f>
+        <v>1.36</v>
+      </c>
       <c r="AB14" t="s">
         <v>8</v>
       </c>
@@ -4105,6 +4141,10 @@
       <c r="Q15">
         <v>2</v>
       </c>
+      <c r="R15">
+        <f>ROUND(AVERAGE(D15:Q15),2)</f>
+        <v>2.0699999999999998</v>
+      </c>
       <c r="AB15" t="s">
         <v>9</v>
       </c>
@@ -4174,6 +4214,10 @@
       </c>
       <c r="Q16">
         <v>2</v>
+      </c>
+      <c r="R16">
+        <f>ROUND(AVERAGE(D16:Q16),2)</f>
+        <v>1.36</v>
       </c>
       <c r="AB16" t="s">
         <v>10</v>

</xml_diff>